<commit_message>
Add converting from guid to UserFriendlyEncodeBase64 string and vice versa extension. (will use if for security), we will do the same for int, long, byte
</commit_message>
<xml_diff>
--- a/Benchmarks/Benchmark/BinarySearchVsLinearSearch/AnalyzeStructureOfSequentialGuid.xlsx
+++ b/Benchmarks/Benchmark/BinarySearchVsLinearSearch/AnalyzeStructureOfSequentialGuid.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sonpham/Projects/Pluralsight/AlgorithmsAndDataStructures/AlgorithmsAndDataStructures_Part2.Explaining/AlgorithmsAndDataStructures_Part2.Benchmarks/BinarySearchVsLinearSearch/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sonpham/Projects/SonPhamProjects/MrpDanu/DDD.MrpDanu/Benchmarks/Benchmark/BinarySearchVsLinearSearch/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1855CE3-CF8D-7A49-BD92-A41EEF29398A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB221A8-3EAE-C44D-9A60-07887F17CAD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -256,7 +256,7 @@
     <t>[9]: {050b32f7-3498-4df8-ac17-08dbe26c72ec}</t>
   </si>
   <si>
-    <t>The "eb" will place first, and then "ec", so we need to compare from the last item to the first item</t>
+    <t>The "eb" will place first, and then "ec", so we need to compare the last component and then the previous component, … please check SqlGuid, CompareTo method for more details.</t>
   </si>
 </sst>
 </file>
@@ -325,10 +325,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -609,7 +609,7 @@
   <dimension ref="A2:I55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+      <selection activeCell="E45" sqref="E45:G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -624,19 +624,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
       <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
       <c r="I2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1021,19 +1021,19 @@
       <c r="I20" s="3"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
       <c r="D22" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
       <c r="I22" s="1" t="s">
         <v>36</v>
       </c>
@@ -1407,141 +1407,141 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" s="6" t="s">
+      <c r="A42" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="6" t="s">
+      <c r="A43" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B43" s="6"/>
-      <c r="C43" s="6"/>
-      <c r="E43" s="6" t="s">
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="E43" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F43" s="6"/>
-      <c r="G43" s="6"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="7" t="s">
+      <c r="A44" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B44" s="7"/>
-      <c r="C44" s="7"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
       <c r="E44" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" s="6" t="s">
+      <c r="A45" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B45" s="6"/>
-      <c r="C45" s="6"/>
-      <c r="E45" s="6" t="s">
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+      <c r="E45" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" s="6" t="s">
+      <c r="A46" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B46" s="6"/>
-      <c r="C46" s="6"/>
-      <c r="E46" s="6" t="s">
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
+      <c r="E46" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" s="6" t="s">
+      <c r="A47" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B47" s="6"/>
-      <c r="C47" s="6"/>
-      <c r="E47" s="6" t="s">
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="E47" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="F47" s="6"/>
-      <c r="G47" s="6"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="6" t="s">
+      <c r="A48" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B48" s="6"/>
-      <c r="C48" s="6"/>
-      <c r="E48" s="6" t="s">
+      <c r="B48" s="7"/>
+      <c r="C48" s="7"/>
+      <c r="E48" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="F48" s="6"/>
-      <c r="G48" s="6"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="6" t="s">
+      <c r="A49" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B49" s="6"/>
-      <c r="C49" s="6"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
       <c r="E49" s="5" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="6" t="s">
+      <c r="A50" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B50" s="6"/>
-      <c r="C50" s="6"/>
-      <c r="E50" s="6" t="s">
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
+      <c r="E50" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="F50" s="6"/>
-      <c r="G50" s="6"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E51" s="6" t="s">
+      <c r="E51" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="F51" s="6"/>
-      <c r="G51" s="6"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="7"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="6" t="s">
+      <c r="A52" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B52" s="6"/>
-      <c r="C52" s="6"/>
-      <c r="E52" s="6" t="s">
+      <c r="B52" s="7"/>
+      <c r="C52" s="7"/>
+      <c r="E52" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="F52" s="6"/>
-      <c r="G52" s="6"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="7"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" s="6" t="s">
+      <c r="A53" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B53" s="6"/>
-      <c r="C53" s="6"/>
-      <c r="E53" s="6" t="s">
+      <c r="B53" s="7"/>
+      <c r="C53" s="7"/>
+      <c r="E53" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F53" s="6"/>
-      <c r="G53" s="6"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="7"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
@@ -1550,6 +1550,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="A42:G42"/>
+    <mergeCell ref="E50:G50"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="A22:C22"/>
@@ -1566,14 +1574,6 @@
     <mergeCell ref="A53:C53"/>
     <mergeCell ref="E45:G45"/>
     <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="A42:G42"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="E43:G43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>